<commit_message>
harmonize tag TANs between templates
</commit_message>
<xml_diff>
--- a/templates/community/FAIRagro/Agronomy_-_Plant_material_sampling/Agronomy_-_Plant_material_sampling_v1.0.0.xlsx
+++ b/templates/community/FAIRagro/Agronomy_-_Plant_material_sampling/Agronomy_-_Plant_material_sampling_v1.0.0.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0460A77-5E0E-4A23-8644-7649331D53CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01515F5D-5265-48C1-BA9D-97B8399A6711}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2196" yWindow="2196" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="isa_template" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="70">
   <si>
     <t>TEMPLATE</t>
   </si>
@@ -94,9 +94,6 @@
     <t>plant material</t>
   </si>
   <si>
-    <t>sampling</t>
-  </si>
-  <si>
     <t>Tags Term Accession Number</t>
   </si>
   <si>
@@ -109,9 +106,6 @@
     <t>http://purl.obolibrary.org/obo/FOODON_00004331</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/C_6774</t>
-  </si>
-  <si>
     <t>Tags Term Source REF</t>
   </si>
   <si>
@@ -239,6 +233,12 @@
   </si>
   <si>
     <t>Agronomy - Plant material sampling</t>
+  </si>
+  <si>
+    <t>Sampling</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/NCIT_C25662</t>
   </si>
 </sst>
 </file>
@@ -278,7 +278,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -630,18 +630,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -649,15 +649,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -665,7 +665,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -673,7 +673,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -681,7 +681,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -689,32 +689,32 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -728,149 +728,143 @@
         <v>20</v>
       </c>
       <c r="E13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="B14" t="s">
         <v>22</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>23</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>24</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>25</v>
       </c>
-      <c r="E14" t="s">
+      <c r="B15" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="C15" t="s">
         <v>27</v>
       </c>
-      <c r="B15" t="s">
+      <c r="D15" t="s">
         <v>28</v>
       </c>
-      <c r="C15" t="s">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>29</v>
       </c>
-      <c r="D15" t="s">
+      <c r="B16" t="s">
         <v>30</v>
       </c>
-      <c r="E15" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="D16" t="s">
         <v>31</v>
       </c>
-      <c r="B16" t="s">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>32</v>
       </c>
-      <c r="D16" t="s">
+      <c r="B17" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="C17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>34</v>
       </c>
-      <c r="B17" t="s">
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>35</v>
       </c>
-      <c r="C17" t="s">
-        <v>35</v>
-      </c>
-      <c r="D17" t="s">
-        <v>35</v>
-      </c>
-      <c r="E17" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="B19" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>37</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>39</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>41</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>43</v>
       </c>
-      <c r="B22" t="s">
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="B30" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>52</v>
-      </c>
-      <c r="B30" t="s">
-        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -885,94 +879,94 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" t="s">
         <v>54</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>55</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>56</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>57</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>58</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>59</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>60</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>61</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>62</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>63</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>64</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>65</v>
       </c>
-      <c r="M1" t="s">
-        <v>66</v>
-      </c>
-      <c r="N1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="K2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="L2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="M2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="N2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>